<commit_message>
UserInputSystem wasd->moveables, recording clicks and double clicks, PhysicsSystem started.
</commit_message>
<xml_diff>
--- a/doc/todolist.xlsx
+++ b/doc/todolist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Camera Tracking</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>Switching State</t>
-  </si>
-  <si>
-    <t>Should different states use different coordinators? Or should entities simply be added/removed from the coordinator and systems deactivated?
-Should the texture manager be moved from Coordinator -&gt; Some new state manager?
-Probably want textures not in use to be removed from memory ... but maybe not. I don't use many textures (yet).
-How to tell when textures won't be needed for a long time?</t>
   </si>
   <si>
     <t>Do a while(SDL Event) and pass it all to a new entity. Entity should be an "event"</t>
@@ -123,6 +117,19 @@
     <t>Inspiration: region system from Rimworld. Break the world up into 16 by 16 tile blocks. Instead of updating attributes for every tile
  every frame, each block will have a flag indicating that the block needs to be updated. Then every tile inside a block is updated. 
 Use this for when to generate new edges for raytracing.</t>
+  </si>
+  <si>
+    <t>Should different states use different coordinators? Or should entities simply be added/removed from the coordinator and systems deactivated?
+Should the texture manager be moved from Coordinator -&gt; Some new state manager?
+Probably want textures not in use to be removed from memory ... but maybe not. I don't use many textures (yet).
+How to tell when textures won't be needed for a long time?
+Extract events + their data from the coordinator and store somewhere else between states.</t>
+  </si>
+  <si>
+    <t>Multithreading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Render system and camera system need multithreading </t>
   </si>
 </sst>
 </file>
@@ -467,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +500,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,105 +511,113 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Demo nlohmann JSON for save files
</commit_message>
<xml_diff>
--- a/doc/todolist.xlsx
+++ b/doc/todolist.xlsx
@@ -28,9 +28,6 @@
     <t>Save/Load System</t>
   </si>
   <si>
-    <t>Self explanatory. Idea: Use JSON to offload all entities in the game to a file and any other state held by the Coordinator.</t>
-  </si>
-  <si>
     <t>Pathfinding</t>
   </si>
   <si>
@@ -129,7 +126,16 @@
     <t>Multithreading</t>
   </si>
   <si>
-    <t xml:space="preserve">Render system and camera system need multithreading </t>
+    <t>Self explanatory. Idea: Use JSON to offload all entities in the game to a file and any other state held by the Coordinator.
+In Progress: using nlohmann json library for json. 
+Plan: Have a "saveable" component which marks entities as saveable. Have SaveSystem which responds to SaveEvent -&gt;
+Go through all saveable entities, call Coordinator getAllData, and dump to JSON file.</t>
+  </si>
+  <si>
+    <t>Render system and camera system need multithreading 
+Done: ComponentArrays are mutex locked.
+Todo: ComponentArrays should allow check out of individual components rather than block entire array for one index being checked out. Have a "master" lock for when components are being added/deleted (the indexes themselves are moving around) vs an individual lock for each entry in the array. 
+Todo: Actually use more than one thread.</t>
   </si>
 </sst>
 </file>
@@ -477,7 +483,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,28 +506,28 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>32</v>
@@ -529,95 +535,95 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reworked multithreaded ecs engine. todo list. collision system underway
</commit_message>
<xml_diff>
--- a/doc/todolist.xlsx
+++ b/doc/todolist.xlsx
@@ -8,13 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Camera Tracking</t>
   </si>
@@ -132,7 +136,61 @@
 Go through all saveable entities, call Coordinator getAllData, and dump to JSON file.</t>
   </si>
   <si>
-    <t>Render system and camera system need multithreading 
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Verification</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Faction System</t>
+  </si>
+  <si>
+    <t>Dwellers have factional preferences. Factions exist based on critical mass of dwellers with a preference. Happiness is combination of personal needs and factional fulfillment. High priority as could be a selling feature, differentiator from DF or Rimworld.</t>
+  </si>
+  <si>
+    <t>Multiple sprites per renderable</t>
+  </si>
+  <si>
+    <t>Select objects</t>
+  </si>
+  <si>
+    <t>Objects can be clicked on. Will display some information depending on context.</t>
+  </si>
+  <si>
+    <t>For changing orientation, animations, etc. Have "active sprites" - a vector of sprites that is iterated through per configurable time interval. Multiple can be active at a time. "Walking left" "Running left" "using hands" "taking damage"</t>
+  </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>Track which components and entity has</t>
+  </si>
+  <si>
+    <t>Need a better solution than checking for each component for each entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 Done: ComponentArrays are mutex locked.
 Todo: ComponentArrays should allow check out of individual components rather than block entire array for one index being checked out. Have a "master" lock for when components are being added/deleted (the indexes themselves are moving around) vs an individual lock for each entry in the array. 
 Todo: Actually use more than one thread.</t>
@@ -171,16 +229,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -480,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,139 +621,464 @@
     <col min="1" max="1" width="33.5703125" customWidth="1"/>
     <col min="2" max="2" width="117.42578125" customWidth="1"/>
     <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1"/>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>"In Work"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Working">
+      <formula>NOT(ISERROR(SEARCH("Working",C1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"Todo"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Verification"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576 E1">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>